<commit_message>
Burndown chart and work breakdown update
</commit_message>
<xml_diff>
--- a/Project_Management/Sprint1/Burndown chart.xlsx
+++ b/Project_Management/Sprint1/Burndown chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27016"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unlpt-my.sharepoint.com/personal/tco_sousa_fct_unl_pt/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgsi\IdeaProjects\SE2324_63191_63324-62654_63069_62551_62482\Project_Management\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E7A4A98-94BE-47C0-9172-A1C6811B492C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA77148-6900-437F-BC5C-CB15789C74C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -74,48 +74,6 @@
     <t>Day 7</t>
   </si>
   <si>
-    <t>Create User Stories for functionalities.</t>
-  </si>
-  <si>
-    <t>Create AuthorInformationTab extending FieldsEditorTab.</t>
-  </si>
-  <si>
-    <t>Create Fields for AuthorInformationTab and display them in it.</t>
-  </si>
-  <si>
-    <t>Find proper data extraction API (Wikidata-Toolkit chosen).</t>
-  </si>
-  <si>
-    <t>Create dynamic group and subgroup creation functionality.</t>
-  </si>
-  <si>
-    <t>Study and examine Wikidata API code.</t>
-  </si>
-  <si>
-    <t>Make parser for Author Name and for Time Value.</t>
-  </si>
-  <si>
-    <t>Make parser for Link to get title from Wikidata.</t>
-  </si>
-  <si>
-    <t>Create WikidataFetcher data extraction logic.</t>
-  </si>
-  <si>
-    <t>Update standard fields to display.</t>
-  </si>
-  <si>
-    <t>Implement EntryBasedParserFetcher interface functions in WikidataFetcher.</t>
-  </si>
-  <si>
-    <t>Create tests for WikidataFetcher (first functionality).</t>
-  </si>
-  <si>
-    <t>Create tests for GroupTreeViewModel (second functionality).</t>
-  </si>
-  <si>
-    <t>Record functionalities demonstration video.</t>
-  </si>
-  <si>
     <t>Completed Effort</t>
   </si>
   <si>
@@ -123,6 +81,21 @@
   </si>
   <si>
     <t>Ideal Burndown</t>
+  </si>
+  <si>
+    <t>Set up the gitHub repository</t>
+  </si>
+  <si>
+    <t>Set up the game</t>
+  </si>
+  <si>
+    <t>Test the game</t>
+  </si>
+  <si>
+    <t>Prepare the structure of future scrums, burndown charts and sprints</t>
+  </si>
+  <si>
+    <t>First quick look at the code</t>
   </si>
 </sst>
 </file>
@@ -133,7 +106,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -460,60 +433,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -627,17 +572,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -663,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -683,16 +617,109 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -700,130 +727,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -850,7 +753,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -912,7 +815,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -928,14 +831,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$20:$C$20</c:f>
+              <c:f>'Burndown Chart'!$B$11:$C$11</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Completed Effort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Record functionalities demonstration video.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -952,7 +852,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$20:$K$20</c:f>
+              <c:f>'Burndown Chart'!$D$11:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -969,13 +869,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1010,14 +910,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$21:$C$21</c:f>
+              <c:f>'Burndown Chart'!$B$12:$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Remaining Effort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Record functionalities demonstration video.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1080,7 +977,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$21:$K$21</c:f>
+              <c:f>'Burndown Chart'!$D$12:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1097,16 +994,16 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1123,14 +1020,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$22:$C$22</c:f>
+              <c:f>'Burndown Chart'!$B$13:$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Ideal Burndown</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Record functionalities demonstration video.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1181,7 +1075,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$22:$K$22</c:f>
+              <c:f>'Burndown Chart'!$D$13:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1273,7 +1167,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1048433599"/>
@@ -1357,7 +1251,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1389,7 +1283,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1048432767"/>
@@ -1431,7 +1325,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1468,7 +1362,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2041,13 +1935,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>16807</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>180414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>177054</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2084,7 +1978,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>129599</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>53670</xdr:rowOff>
+      <xdr:rowOff>35741</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2130,14 +2024,14 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2479,460 +2373,309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L22"/>
+  <dimension ref="B3:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15"/>
-    <row r="2" spans="2:11" ht="15"/>
-    <row r="3" spans="2:11" ht="15">
-      <c r="B3" s="32" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="34"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="33"/>
     </row>
-    <row r="4" spans="2:11" ht="15">
-      <c r="B4" s="24" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="27">
-        <v>44546</v>
-      </c>
-      <c r="F4" s="27">
-        <v>44547</v>
-      </c>
-      <c r="G4" s="27">
-        <v>44548</v>
-      </c>
-      <c r="H4" s="27">
-        <v>44549</v>
-      </c>
-      <c r="I4" s="27">
-        <v>44550</v>
-      </c>
-      <c r="J4" s="27">
-        <v>44551</v>
-      </c>
-      <c r="K4" s="28">
-        <v>44552</v>
+      <c r="E4" s="14">
+        <v>45215</v>
+      </c>
+      <c r="F4" s="14">
+        <v>45216</v>
+      </c>
+      <c r="G4" s="14">
+        <v>45217</v>
+      </c>
+      <c r="H4" s="14">
+        <v>45218</v>
+      </c>
+      <c r="I4" s="14">
+        <v>45219</v>
+      </c>
+      <c r="J4" s="14">
+        <v>45220</v>
+      </c>
+      <c r="K4" s="14">
+        <v>45221</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="15">
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="31" t="s">
+    <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="37"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="52" t="s">
+      <c r="H5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="52" t="s">
+      <c r="I5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="52" t="s">
+      <c r="J5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="15">
-      <c r="B6" s="35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="16">
         <v>1</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="50">
-        <v>1</v>
-      </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="41"/>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="27">
+        <v>4</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20">
+        <v>2</v>
+      </c>
+      <c r="I6" s="20">
+        <v>2</v>
+      </c>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21"/>
     </row>
-    <row r="7" spans="2:11" ht="15">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
         <v>2</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="8">
-        <v>1</v>
-      </c>
-      <c r="E7" s="42"/>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="7">
+        <v>3</v>
+      </c>
+      <c r="E7" s="22"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="43"/>
+      <c r="K7" s="23"/>
     </row>
-    <row r="8" spans="2:11" ht="15">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="6">
         <v>3</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="8">
-        <v>2</v>
-      </c>
-      <c r="E8" s="44"/>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7">
+        <v>5</v>
+      </c>
+      <c r="E8" s="24"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="43"/>
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
+      <c r="K8" s="23"/>
     </row>
-    <row r="9" spans="2:11" ht="15">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
         <v>4</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="8">
-        <v>1</v>
-      </c>
-      <c r="E9" s="45"/>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7">
+        <v>3</v>
+      </c>
+      <c r="E9" s="25"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1">
+        <v>2</v>
+      </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="43"/>
+      <c r="K9" s="23"/>
     </row>
-    <row r="10" spans="2:11" ht="15">
+    <row r="10" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
         <v>5</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="8">
-        <v>2</v>
-      </c>
-      <c r="E10" s="46"/>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="7">
+        <v>5</v>
+      </c>
+      <c r="E10" s="26"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="43"/>
+      <c r="J10" s="1">
+        <v>2</v>
+      </c>
+      <c r="K10" s="23"/>
     </row>
-    <row r="11" spans="2:11" ht="15">
-      <c r="B11" s="6">
-        <v>6</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>17</v>
-      </c>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="43"/>
       <c r="D11" s="8">
-        <v>1</v>
-      </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="43"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="29">
+        <f>SUM(E6:E10)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="29">
+        <f>SUM(F6:F10)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="29">
+        <f>SUM(G6:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="29">
+        <f>SUM(H6:H10)</f>
+        <v>2</v>
+      </c>
+      <c r="I11" s="29">
+        <f>SUM(I6:I10)</f>
+        <v>10</v>
+      </c>
+      <c r="J11" s="29">
+        <f>SUM(J6:J10)</f>
+        <v>4</v>
+      </c>
+      <c r="K11" s="30">
+        <f>SUM(K6:K10)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="2:11" ht="15">
-      <c r="B12" s="6">
-        <v>7</v>
-      </c>
-      <c r="C12" s="7" t="s">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="4">
+        <f>SUM(D6:D11)</f>
+        <v>20</v>
+      </c>
+      <c r="E12" s="5">
+        <f>D12-SUM(E6:E10)</f>
+        <v>20</v>
+      </c>
+      <c r="F12" s="3">
+        <f>E12-SUM(F6:F10)</f>
+        <v>20</v>
+      </c>
+      <c r="G12" s="3">
+        <f>F12-SUM(G6:G10)</f>
+        <v>20</v>
+      </c>
+      <c r="H12" s="3">
+        <f>G12-SUM(H6:H10)</f>
         <v>18</v>
       </c>
-      <c r="D12" s="8">
-        <v>1</v>
-      </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="43"/>
+      <c r="I12" s="3">
+        <f>H12-SUM(I6:I10)</f>
+        <v>8</v>
+      </c>
+      <c r="J12" s="2">
+        <f>I12-SUM(J6:J10)</f>
+        <v>4</v>
+      </c>
+      <c r="K12" s="17">
+        <f>J12-SUM(K6:K10)</f>
+        <v>4</v>
+      </c>
     </row>
-    <row r="13" spans="2:11" ht="15">
-      <c r="B13" s="6">
-        <v>8</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="8">
-        <v>1</v>
-      </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="43"/>
-    </row>
-    <row r="14" spans="2:11" ht="15">
-      <c r="B14" s="6">
-        <v>9</v>
-      </c>
-      <c r="C14" s="7" t="s">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="41"/>
+      <c r="D13" s="9">
+        <f>D12</f>
         <v>20</v>
       </c>
-      <c r="D14" s="8">
-        <v>4</v>
-      </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="43"/>
-    </row>
-    <row r="15" spans="2:11" ht="15">
-      <c r="B15" s="6">
-        <v>10</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="8">
-        <v>1</v>
-      </c>
-      <c r="E15" s="46"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="43"/>
-    </row>
-    <row r="16" spans="2:11" ht="15">
-      <c r="B16" s="6">
-        <v>11</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="8">
-        <v>2</v>
-      </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="43"/>
-    </row>
-    <row r="17" spans="2:12" ht="15">
-      <c r="B17" s="6">
-        <v>12</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="8">
-        <v>1</v>
-      </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="43"/>
-    </row>
-    <row r="18" spans="2:12" ht="15">
-      <c r="B18" s="6">
-        <v>13</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="8">
-        <v>1</v>
-      </c>
-      <c r="E18" s="46"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="43"/>
-    </row>
-    <row r="19" spans="2:12" ht="15">
-      <c r="B19" s="22">
-        <v>14</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="51">
-        <v>1</v>
-      </c>
-      <c r="E19" s="47"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="49"/>
-    </row>
-    <row r="20" spans="2:12" ht="15">
-      <c r="B20" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13">
-        <v>0</v>
-      </c>
-      <c r="E20" s="53">
-        <f t="shared" ref="E20:K20" si="0">SUM(E6:E19)</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L20" s="21"/>
-    </row>
-    <row r="21" spans="2:12" ht="15">
-      <c r="B21" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="4">
-        <f>SUM(D6:D20)</f>
-        <v>20</v>
-      </c>
-      <c r="E21" s="5">
-        <f t="shared" ref="E21:K21" si="1">D21-SUM(E6:E19)</f>
-        <v>20</v>
-      </c>
-      <c r="F21" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="G21" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="H21" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="I21" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="J21" s="2">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="K21" s="37">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="15">
-      <c r="B22" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="17">
-        <f>D21</f>
-        <v>20</v>
-      </c>
-      <c r="E22" s="18">
-        <f>$D$22-($D$22/7*1)</f>
+      <c r="E13" s="10">
+        <f>$D$13-($D$13/7*1)</f>
         <v>17.142857142857142</v>
       </c>
-      <c r="F22" s="19">
-        <f>$D$22-($D$22/7*2)</f>
+      <c r="F13" s="11">
+        <f>$D$13-($D$13/7*2)</f>
         <v>14.285714285714285</v>
       </c>
-      <c r="G22" s="19">
-        <f>$D$22-($D$22/7*3)</f>
+      <c r="G13" s="11">
+        <f>$D$13-($D$13/7*3)</f>
         <v>11.428571428571429</v>
       </c>
-      <c r="H22" s="19">
-        <f>$D$22-($D$22/7*4)</f>
+      <c r="H13" s="11">
+        <f>$D$13-($D$13/7*4)</f>
         <v>8.5714285714285712</v>
       </c>
-      <c r="I22" s="19">
-        <f>$D$22-($D$22/7*5)</f>
+      <c r="I13" s="11">
+        <f>$D$13-($D$13/7*5)</f>
         <v>5.7142857142857135</v>
       </c>
-      <c r="J22" s="19">
-        <f>$D$22-($D$22/7*6)</f>
+      <c r="J13" s="11">
+        <f>$D$13-($D$13/7*6)</f>
         <v>2.8571428571428577</v>
       </c>
-      <c r="K22" s="20">
-        <f>$D$22-($D$22/7*7)</f>
+      <c r="K13" s="12">
+        <f>$D$13-($D$13/7*7)</f>
         <v>0</v>
       </c>
     </row>
@@ -2941,9 +2684,9 @@
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2953,21 +2696,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EA6DE6520660014F909ED4D690581D99" ma:contentTypeVersion="0" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="0963fafc81e756851797ef866a65fefe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a86f9ef69356bc5d2158216095de652a">
     <xsd:element name="properties">
@@ -3081,14 +2809,50 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{738E5DA7-A17B-4FAD-9104-2B5232F8C5EE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{612D18BE-71E8-4EBC-AC22-EB1D6ECED47C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BF93E43-0769-4CD0-A2DD-49C5CE2CDD2F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BF93E43-0769-4CD0-A2DD-49C5CE2CDD2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{612D18BE-71E8-4EBC-AC22-EB1D6ECED47C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{738E5DA7-A17B-4FAD-9104-2B5232F8C5EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Burndown chart 1 update
</commit_message>
<xml_diff>
--- a/Project_Management/Sprint1/Burndown chart.xlsx
+++ b/Project_Management/Sprint1/Burndown chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgsi\IdeaProjects\SE2324_63191_63324-62654_63069_62551_62482\Project_Management\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA77148-6900-437F-BC5C-CB15789C74C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CE6728-A37C-4F80-8DA8-9746F2EC515F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>First quick look at the code</t>
+  </si>
+  <si>
+    <t>Define User Stories</t>
   </si>
 </sst>
 </file>
@@ -308,19 +311,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -593,11 +583,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -620,46 +623,49 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -674,19 +680,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
@@ -695,39 +701,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,7 +838,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$11:$C$11</c:f>
+              <c:f>'Burndown Chart'!$B$12:$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -852,7 +859,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$11:$K$11</c:f>
+              <c:f>'Burndown Chart'!$D$12:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -860,22 +867,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -910,7 +917,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$12:$C$12</c:f>
+              <c:f>'Burndown Chart'!$B$13:$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -977,7 +984,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$12:$K$12</c:f>
+              <c:f>'Burndown Chart'!$D$13:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
@@ -985,25 +992,25 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1020,7 +1027,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$13:$C$13</c:f>
+              <c:f>'Burndown Chart'!$B$14:$C$14</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1075,7 +1082,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$13:$K$13</c:f>
+              <c:f>'Burndown Chart'!$D$14:$K$14</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1935,13 +1942,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>16807</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>180414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>177054</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1965,112 +1972,6 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>357867</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>160563</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>129599</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>35741</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFB13DAA-0C66-35DA-DF84-0E4429AC8663}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{52BFCA64-3DDA-4711-BDFA-D2973C7C7C4B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="21576292">
-          <a:off x="14616792" y="922563"/>
-          <a:ext cx="2381582" cy="2369607"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC6CD824-D46B-AF55-82FE-B64B07E184D5}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{CFB13DAA-0C66-35DA-DF84-0E4429AC8663}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12296775" y="2657475"/>
-          <a:ext cx="7191375" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2373,10 +2274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:K13"/>
+  <dimension ref="B3:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2413,25 +2314,25 @@
         <v>3</v>
       </c>
       <c r="E4" s="14">
-        <v>45215</v>
+        <v>45222</v>
       </c>
       <c r="F4" s="14">
-        <v>45216</v>
+        <v>45223</v>
       </c>
       <c r="G4" s="14">
-        <v>45217</v>
+        <v>45224</v>
       </c>
       <c r="H4" s="14">
-        <v>45218</v>
+        <v>45225</v>
       </c>
       <c r="I4" s="14">
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="J4" s="14">
-        <v>45220</v>
+        <v>45227</v>
       </c>
       <c r="K4" s="14">
-        <v>45221</v>
+        <v>45228</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2466,21 +2367,19 @@
       <c r="B6" s="16">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="46" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="27">
         <v>4</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="19">
+        <v>4</v>
+      </c>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
-      <c r="H6" s="20">
-        <v>2</v>
-      </c>
-      <c r="I6" s="20">
-        <v>2</v>
-      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="21"/>
     </row>
@@ -2488,19 +2387,19 @@
       <c r="B7" s="6">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="44" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="7">
         <v>3</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="22">
+        <v>3</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1">
-        <v>3</v>
-      </c>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="23"/>
     </row>
@@ -2508,174 +2407,202 @@
       <c r="B8" s="6">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="47" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="7">
-        <v>5</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="E8" s="24">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1">
-        <v>3</v>
-      </c>
-      <c r="J8" s="1">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J8" s="1"/>
       <c r="K8" s="23"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="47" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="7">
         <v>3</v>
       </c>
       <c r="E9" s="25"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="23"/>
     </row>
-    <row r="10" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="6">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="47" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="7">
-        <v>5</v>
-      </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="E10" s="26">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1">
-        <v>2</v>
-      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1"/>
       <c r="K10" s="23"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="29">
-        <f>SUM(E6:E10)</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="29">
-        <f>SUM(F6:F10)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="29">
-        <f>SUM(G6:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="29">
-        <f>SUM(H6:H10)</f>
+    <row r="11" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="6">
+        <v>6</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="7">
         <v>2</v>
       </c>
-      <c r="I11" s="29">
-        <f>SUM(I6:I10)</f>
-        <v>10</v>
-      </c>
-      <c r="J11" s="29">
-        <f>SUM(J6:J10)</f>
-        <v>4</v>
-      </c>
-      <c r="K11" s="30">
-        <f>SUM(K6:K10)</f>
-        <v>0</v>
-      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="4">
-        <f>SUM(D6:D11)</f>
-        <v>20</v>
-      </c>
-      <c r="E12" s="5">
-        <f>D12-SUM(E6:E10)</f>
-        <v>20</v>
-      </c>
-      <c r="F12" s="3">
-        <f>E12-SUM(F6:F10)</f>
-        <v>20</v>
-      </c>
-      <c r="G12" s="3">
-        <f>F12-SUM(G6:G10)</f>
-        <v>20</v>
-      </c>
-      <c r="H12" s="3">
-        <f>G12-SUM(H6:H10)</f>
-        <v>18</v>
-      </c>
-      <c r="I12" s="3">
-        <f>H12-SUM(I6:I10)</f>
-        <v>8</v>
-      </c>
-      <c r="J12" s="2">
-        <f>I12-SUM(J6:J10)</f>
+      <c r="B12" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="29">
+        <f t="shared" ref="E12:K12" si="0">SUM(E6:E11)</f>
+        <v>11</v>
+      </c>
+      <c r="F12" s="29">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K12" s="17">
-        <f>J12-SUM(K6:K10)</f>
-        <v>4</v>
+      <c r="G12" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="29">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J12" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="4">
+        <f>SUM(D6:D12)</f>
+        <v>20</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" ref="E13:K13" si="1">D13-SUM(E6:E11)</f>
+        <v>9</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="9">
-        <f>D12</f>
+      <c r="C14" s="41"/>
+      <c r="D14" s="9">
+        <f>D13</f>
         <v>20</v>
       </c>
-      <c r="E13" s="10">
-        <f>$D$13-($D$13/7*1)</f>
+      <c r="E14" s="10">
+        <f>$D$14-($D$14/7*1)</f>
         <v>17.142857142857142</v>
       </c>
-      <c r="F13" s="11">
-        <f>$D$13-($D$13/7*2)</f>
+      <c r="F14" s="11">
+        <f>$D$14-($D$14/7*2)</f>
         <v>14.285714285714285</v>
       </c>
-      <c r="G13" s="11">
-        <f>$D$13-($D$13/7*3)</f>
+      <c r="G14" s="11">
+        <f>$D$14-($D$14/7*3)</f>
         <v>11.428571428571429</v>
       </c>
-      <c r="H13" s="11">
-        <f>$D$13-($D$13/7*4)</f>
+      <c r="H14" s="11">
+        <f>$D$14-($D$14/7*4)</f>
         <v>8.5714285714285712</v>
       </c>
-      <c r="I13" s="11">
-        <f>$D$13-($D$13/7*5)</f>
+      <c r="I14" s="11">
+        <f>$D$14-($D$14/7*5)</f>
         <v>5.7142857142857135</v>
       </c>
-      <c r="J13" s="11">
-        <f>$D$13-($D$13/7*6)</f>
+      <c r="J14" s="11">
+        <f>$D$14-($D$14/7*6)</f>
         <v>2.8571428571428577</v>
       </c>
-      <c r="K13" s="12">
-        <f>$D$13-($D$13/7*7)</f>
+      <c r="K14" s="12">
+        <f>$D$14-($D$14/7*7)</f>
         <v>0</v>
       </c>
     </row>
@@ -2684,9 +2611,9 @@
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2696,6 +2623,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EA6DE6520660014F909ED4D690581D99" ma:contentTypeVersion="0" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="0963fafc81e756851797ef866a65fefe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a86f9ef69356bc5d2158216095de652a">
     <xsd:element name="properties">
@@ -2809,33 +2751,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{612D18BE-71E8-4EBC-AC22-EB1D6ECED47C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{738E5DA7-A17B-4FAD-9104-2B5232F8C5EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2850,9 +2769,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{738E5DA7-A17B-4FAD-9104-2B5232F8C5EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{612D18BE-71E8-4EBC-AC22-EB1D6ECED47C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>